<commit_message>
Update Levi‘s CMS Operation&Maintenance Request List_CN.xlsx
</commit_message>
<xml_diff>
--- a/2019/总体管理/Levi‘s CMS Operation&Maintenance Request List_CN.xlsx
+++ b/2019/总体管理/Levi‘s CMS Operation&Maintenance Request List_CN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File Server\Tree Sapling\03 Levi's\gitCube-levisProject\2019\总体管理\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DB446B-53EF-452F-8D93-E017F398963B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E2EBFA-6141-42FB-A0A3-AE07A8157E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="972" yWindow="-108" windowWidth="22176" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>*</t>
   </si>
@@ -458,6 +458,24 @@
     <rPh sb="2" eb="3">
       <t>チュウ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">【2019/11/01】
+追加投放内容
+链接：https://pan.baidu.com/s/1yFZGtjNCZSnff0Domx2nEQ
+提取码：7hua
+（仅播放有分割线的视频，另一个不投放）
+网络确认完成，新内容已投
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>任秋凤</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>郭文博</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -747,7 +765,7 @@
     <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -849,28 +867,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="17" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -897,14 +895,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="181" fontId="16" fillId="8" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -921,16 +911,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="17" fillId="8" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -941,7 +939,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3456,11 +3466,11 @@
   <dimension ref="A1:AD74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="F2" sqref="F2"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="12"/>
@@ -3647,70 +3657,70 @@
       <c r="AD4" s="25"/>
     </row>
     <row r="5" spans="1:30" s="1" customFormat="1" ht="26.4">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="39" t="s">
+      <c r="P5" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="41" t="s">
+      <c r="Q5" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="42" t="s">
+      <c r="R5" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="42" t="s">
+      <c r="S5" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="T5" s="42" t="s">
+      <c r="T5" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="U5" s="43" t="s">
+      <c r="U5" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="44"/>
+      <c r="V5" s="50"/>
       <c r="W5" s="19" t="s">
         <v>0</v>
       </c>
@@ -3733,69 +3743,69 @@
       <c r="AD5" s="21"/>
     </row>
     <row r="6" spans="1:30" s="2" customFormat="1" ht="84">
-      <c r="A6" s="45">
+      <c r="A6" s="38">
         <f>ROW()-5</f>
         <v>1</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="47" t="s">
+      <c r="K6" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="47" t="s">
+      <c r="L6" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="M6" s="47" t="s">
+      <c r="M6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="O6" s="48" t="s">
+      <c r="O6" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="P6" s="49" t="s">
+      <c r="P6" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="Q6" s="50" t="s">
+      <c r="Q6" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="R6" s="47" t="s">
+      <c r="R6" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="48" t="s">
+      <c r="S6" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="T6" s="51" t="s">
+      <c r="T6" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="U6" s="52"/>
-      <c r="V6" s="53"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="48"/>
       <c r="W6" s="16"/>
       <c r="X6" s="21"/>
       <c r="Y6" s="21"/>
@@ -3806,69 +3816,69 @@
       <c r="AD6" s="23"/>
     </row>
     <row r="7" spans="1:30" s="2" customFormat="1" ht="84">
-      <c r="A7" s="45">
+      <c r="A7" s="38">
         <f t="shared" ref="A7:A70" si="0">ROW()-5</f>
         <v>2</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="G7" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="K7" s="47" t="s">
+      <c r="K7" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="47" t="s">
+      <c r="L7" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="47" t="s">
+      <c r="M7" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="47" t="s">
+      <c r="N7" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="O7" s="48" t="s">
+      <c r="O7" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="P7" s="54" t="s">
+      <c r="P7" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" s="50" t="s">
+      <c r="Q7" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="R7" s="51">
+      <c r="R7" s="43">
         <v>43753</v>
       </c>
-      <c r="S7" s="48" t="s">
+      <c r="S7" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="T7" s="48" t="s">
+      <c r="T7" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="U7" s="52"/>
-      <c r="V7" s="53"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="48"/>
       <c r="W7" s="16"/>
       <c r="X7" s="21" t="s">
         <v>4</v>
@@ -3889,69 +3899,69 @@
       <c r="AD7" s="23"/>
     </row>
     <row r="8" spans="1:30" s="2" customFormat="1" ht="84">
-      <c r="A8" s="45">
+      <c r="A8" s="38">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="47" t="s">
+      <c r="K8" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="47" t="s">
+      <c r="L8" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="M8" s="47" t="s">
+      <c r="M8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="47" t="s">
+      <c r="N8" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="48" t="s">
+      <c r="O8" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="P8" s="49" t="s">
+      <c r="P8" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="Q8" s="50" t="s">
+      <c r="Q8" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="R8" s="47" t="s">
+      <c r="R8" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="S8" s="48" t="s">
+      <c r="S8" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="T8" s="51" t="s">
+      <c r="T8" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="U8" s="52"/>
-      <c r="V8" s="53"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="48"/>
       <c r="W8" s="16"/>
       <c r="X8" s="20" t="s">
         <v>97</v>
@@ -3972,69 +3982,69 @@
       <c r="AD8" s="23"/>
     </row>
     <row r="9" spans="1:30" s="2" customFormat="1" ht="156">
-      <c r="A9" s="45">
+      <c r="A9" s="38">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="47" t="s">
+      <c r="J9" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="47" t="s">
+      <c r="K9" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="47" t="s">
+      <c r="L9" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="47" t="s">
+      <c r="M9" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="N9" s="47" t="s">
+      <c r="N9" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="O9" s="48" t="s">
+      <c r="O9" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="P9" s="49" t="s">
+      <c r="P9" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="Q9" s="50" t="s">
+      <c r="Q9" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="R9" s="51">
+      <c r="R9" s="43">
         <v>43760</v>
       </c>
-      <c r="S9" s="48" t="s">
+      <c r="S9" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="T9" s="48" t="s">
+      <c r="T9" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="U9" s="52"/>
-      <c r="V9" s="53"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="48"/>
       <c r="W9" s="16"/>
       <c r="X9" s="20" t="s">
         <v>95</v>
@@ -4054,62 +4064,70 @@
       <c r="AC9" s="23"/>
       <c r="AD9" s="23"/>
     </row>
-    <row r="10" spans="1:30" s="2" customFormat="1" ht="72">
-      <c r="A10" s="27">
+    <row r="10" spans="1:30" s="2" customFormat="1" ht="108">
+      <c r="A10" s="38">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="I10" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="29" t="s">
+      <c r="J10" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="29" t="s">
+      <c r="L10" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="29" t="s">
+      <c r="N10" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="30" t="s">
+      <c r="O10" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="P10" s="31" t="s">
+      <c r="P10" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="33"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="35"/>
+      <c r="Q10" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="R10" s="43">
+        <v>43770</v>
+      </c>
+      <c r="S10" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="T10" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="U10" s="47"/>
+      <c r="V10" s="48"/>
       <c r="W10" s="16"/>
       <c r="X10" s="20" t="s">
         <v>96</v>
@@ -4146,13 +4164,13 @@
       <c r="M11" s="29"/>
       <c r="N11" s="29"/>
       <c r="O11" s="30"/>
-      <c r="P11" s="31"/>
+      <c r="P11" s="51"/>
       <c r="Q11" s="32"/>
-      <c r="R11" s="33"/>
+      <c r="R11" s="31"/>
       <c r="S11" s="30"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="34"/>
-      <c r="V11" s="35"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="46"/>
       <c r="W11" s="16"/>
       <c r="X11" s="21" t="s">
         <v>5</v>
@@ -4185,13 +4203,13 @@
       <c r="M12" s="29"/>
       <c r="N12" s="29"/>
       <c r="O12" s="30"/>
-      <c r="P12" s="31"/>
+      <c r="P12" s="51"/>
       <c r="Q12" s="32"/>
-      <c r="R12" s="33"/>
+      <c r="R12" s="31"/>
       <c r="S12" s="30"/>
-      <c r="T12" s="33"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="35"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="46"/>
       <c r="W12" s="16"/>
       <c r="X12" s="21" t="s">
         <v>6</v>
@@ -4222,13 +4240,13 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="30"/>
-      <c r="P13" s="31"/>
+      <c r="P13" s="51"/>
       <c r="Q13" s="32"/>
-      <c r="R13" s="33"/>
+      <c r="R13" s="31"/>
       <c r="S13" s="30"/>
-      <c r="T13" s="33"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="35"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="45"/>
+      <c r="V13" s="46"/>
       <c r="W13" s="16"/>
       <c r="X13" s="21"/>
       <c r="Y13" s="21"/>
@@ -4257,13 +4275,13 @@
       <c r="M14" s="29"/>
       <c r="N14" s="29"/>
       <c r="O14" s="30"/>
-      <c r="P14" s="31"/>
+      <c r="P14" s="51"/>
       <c r="Q14" s="32"/>
-      <c r="R14" s="33"/>
+      <c r="R14" s="31"/>
       <c r="S14" s="30"/>
-      <c r="T14" s="33"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="35"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="46"/>
       <c r="W14" s="16"/>
       <c r="X14" s="21"/>
       <c r="Y14" s="21"/>
@@ -4292,13 +4310,13 @@
       <c r="M15" s="29"/>
       <c r="N15" s="29"/>
       <c r="O15" s="30"/>
-      <c r="P15" s="31"/>
+      <c r="P15" s="51"/>
       <c r="Q15" s="32"/>
-      <c r="R15" s="33"/>
+      <c r="R15" s="31"/>
       <c r="S15" s="30"/>
-      <c r="T15" s="33"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="35"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="46"/>
       <c r="W15" s="16"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
@@ -4327,13 +4345,13 @@
       <c r="M16" s="29"/>
       <c r="N16" s="29"/>
       <c r="O16" s="30"/>
-      <c r="P16" s="31"/>
+      <c r="P16" s="51"/>
       <c r="Q16" s="32"/>
-      <c r="R16" s="33"/>
+      <c r="R16" s="31"/>
       <c r="S16" s="30"/>
-      <c r="T16" s="33"/>
-      <c r="U16" s="34"/>
-      <c r="V16" s="35"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="46"/>
       <c r="W16" s="16"/>
       <c r="X16" s="21"/>
       <c r="Y16" s="21"/>
@@ -4362,13 +4380,13 @@
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
       <c r="O17" s="30"/>
-      <c r="P17" s="31"/>
+      <c r="P17" s="51"/>
       <c r="Q17" s="32"/>
-      <c r="R17" s="33"/>
+      <c r="R17" s="31"/>
       <c r="S17" s="30"/>
-      <c r="T17" s="33"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="35"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="46"/>
       <c r="W17" s="16"/>
       <c r="X17" s="21"/>
       <c r="Y17" s="21"/>
@@ -4397,13 +4415,13 @@
       <c r="M18" s="29"/>
       <c r="N18" s="29"/>
       <c r="O18" s="30"/>
-      <c r="P18" s="31"/>
+      <c r="P18" s="51"/>
       <c r="Q18" s="32"/>
-      <c r="R18" s="33"/>
+      <c r="R18" s="31"/>
       <c r="S18" s="30"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="35"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="46"/>
       <c r="W18" s="16"/>
       <c r="X18" s="21"/>
       <c r="Y18" s="21"/>
@@ -4432,13 +4450,13 @@
       <c r="M19" s="29"/>
       <c r="N19" s="29"/>
       <c r="O19" s="30"/>
-      <c r="P19" s="31"/>
+      <c r="P19" s="51"/>
       <c r="Q19" s="32"/>
-      <c r="R19" s="33"/>
+      <c r="R19" s="31"/>
       <c r="S19" s="30"/>
-      <c r="T19" s="33"/>
-      <c r="U19" s="34"/>
-      <c r="V19" s="35"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="46"/>
       <c r="W19" s="16"/>
       <c r="X19" s="21"/>
       <c r="Y19" s="21"/>
@@ -4467,13 +4485,13 @@
       <c r="M20" s="29"/>
       <c r="N20" s="29"/>
       <c r="O20" s="30"/>
-      <c r="P20" s="31"/>
+      <c r="P20" s="51"/>
       <c r="Q20" s="32"/>
-      <c r="R20" s="33"/>
+      <c r="R20" s="31"/>
       <c r="S20" s="30"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="35"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="46"/>
       <c r="W20" s="16"/>
       <c r="X20" s="21"/>
       <c r="Y20" s="21"/>
@@ -4502,13 +4520,13 @@
       <c r="M21" s="29"/>
       <c r="N21" s="29"/>
       <c r="O21" s="30"/>
-      <c r="P21" s="31"/>
+      <c r="P21" s="51"/>
       <c r="Q21" s="32"/>
-      <c r="R21" s="33"/>
+      <c r="R21" s="31"/>
       <c r="S21" s="30"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="35"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="46"/>
       <c r="W21" s="16"/>
       <c r="X21" s="21"/>
       <c r="Y21" s="21"/>
@@ -4537,13 +4555,13 @@
       <c r="M22" s="29"/>
       <c r="N22" s="29"/>
       <c r="O22" s="30"/>
-      <c r="P22" s="31"/>
+      <c r="P22" s="51"/>
       <c r="Q22" s="32"/>
-      <c r="R22" s="33"/>
+      <c r="R22" s="31"/>
       <c r="S22" s="30"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="35"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="46"/>
       <c r="W22" s="16"/>
       <c r="X22" s="21"/>
       <c r="Y22" s="21"/>
@@ -4572,13 +4590,13 @@
       <c r="M23" s="29"/>
       <c r="N23" s="29"/>
       <c r="O23" s="30"/>
-      <c r="P23" s="31"/>
+      <c r="P23" s="51"/>
       <c r="Q23" s="32"/>
-      <c r="R23" s="33"/>
+      <c r="R23" s="31"/>
       <c r="S23" s="30"/>
-      <c r="T23" s="33"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="35"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="46"/>
       <c r="W23" s="16"/>
       <c r="X23" s="21"/>
       <c r="Y23" s="21"/>
@@ -4607,13 +4625,13 @@
       <c r="M24" s="29"/>
       <c r="N24" s="29"/>
       <c r="O24" s="30"/>
-      <c r="P24" s="31"/>
+      <c r="P24" s="51"/>
       <c r="Q24" s="32"/>
-      <c r="R24" s="33"/>
+      <c r="R24" s="31"/>
       <c r="S24" s="30"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="34"/>
-      <c r="V24" s="35"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="46"/>
       <c r="W24" s="16"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="21"/>
@@ -4642,13 +4660,13 @@
       <c r="M25" s="29"/>
       <c r="N25" s="29"/>
       <c r="O25" s="30"/>
-      <c r="P25" s="31"/>
+      <c r="P25" s="51"/>
       <c r="Q25" s="32"/>
-      <c r="R25" s="33"/>
+      <c r="R25" s="31"/>
       <c r="S25" s="30"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="35"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="46"/>
       <c r="W25" s="16"/>
       <c r="X25" s="7"/>
       <c r="Y25" s="7"/>
@@ -4677,13 +4695,13 @@
       <c r="M26" s="29"/>
       <c r="N26" s="29"/>
       <c r="O26" s="30"/>
-      <c r="P26" s="31"/>
+      <c r="P26" s="51"/>
       <c r="Q26" s="32"/>
-      <c r="R26" s="33"/>
+      <c r="R26" s="31"/>
       <c r="S26" s="30"/>
-      <c r="T26" s="33"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="35"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="45"/>
+      <c r="V26" s="46"/>
       <c r="W26" s="16"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
@@ -4712,13 +4730,13 @@
       <c r="M27" s="29"/>
       <c r="N27" s="29"/>
       <c r="O27" s="30"/>
-      <c r="P27" s="31"/>
+      <c r="P27" s="51"/>
       <c r="Q27" s="32"/>
-      <c r="R27" s="33"/>
+      <c r="R27" s="31"/>
       <c r="S27" s="30"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="34"/>
-      <c r="V27" s="35"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="45"/>
+      <c r="V27" s="46"/>
       <c r="W27" s="16"/>
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
@@ -4747,13 +4765,13 @@
       <c r="M28" s="29"/>
       <c r="N28" s="29"/>
       <c r="O28" s="30"/>
-      <c r="P28" s="31"/>
+      <c r="P28" s="51"/>
       <c r="Q28" s="32"/>
-      <c r="R28" s="33"/>
+      <c r="R28" s="31"/>
       <c r="S28" s="30"/>
-      <c r="T28" s="33"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="35"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="46"/>
       <c r="W28" s="24"/>
       <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
@@ -4782,13 +4800,13 @@
       <c r="M29" s="29"/>
       <c r="N29" s="29"/>
       <c r="O29" s="30"/>
-      <c r="P29" s="31"/>
+      <c r="P29" s="51"/>
       <c r="Q29" s="32"/>
-      <c r="R29" s="33"/>
+      <c r="R29" s="31"/>
       <c r="S29" s="30"/>
-      <c r="T29" s="33"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="35"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="46"/>
       <c r="W29" s="24"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
@@ -4817,13 +4835,13 @@
       <c r="M30" s="29"/>
       <c r="N30" s="29"/>
       <c r="O30" s="30"/>
-      <c r="P30" s="31"/>
+      <c r="P30" s="51"/>
       <c r="Q30" s="32"/>
-      <c r="R30" s="33"/>
+      <c r="R30" s="31"/>
       <c r="S30" s="30"/>
-      <c r="T30" s="33"/>
-      <c r="U30" s="34"/>
-      <c r="V30" s="35"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="46"/>
       <c r="W30" s="24"/>
       <c r="X30" s="7"/>
       <c r="Y30" s="7"/>
@@ -4852,13 +4870,13 @@
       <c r="M31" s="29"/>
       <c r="N31" s="29"/>
       <c r="O31" s="30"/>
-      <c r="P31" s="31"/>
+      <c r="P31" s="51"/>
       <c r="Q31" s="32"/>
-      <c r="R31" s="33"/>
+      <c r="R31" s="31"/>
       <c r="S31" s="30"/>
-      <c r="T31" s="33"/>
-      <c r="U31" s="34"/>
-      <c r="V31" s="35"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="46"/>
       <c r="W31" s="24"/>
       <c r="X31" s="7"/>
       <c r="Y31" s="7"/>
@@ -4887,13 +4905,13 @@
       <c r="M32" s="29"/>
       <c r="N32" s="29"/>
       <c r="O32" s="30"/>
-      <c r="P32" s="31"/>
+      <c r="P32" s="51"/>
       <c r="Q32" s="32"/>
-      <c r="R32" s="33"/>
+      <c r="R32" s="31"/>
       <c r="S32" s="30"/>
-      <c r="T32" s="33"/>
-      <c r="U32" s="34"/>
-      <c r="V32" s="35"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="46"/>
       <c r="W32" s="24"/>
       <c r="X32" s="7"/>
       <c r="Y32" s="7"/>
@@ -4922,13 +4940,13 @@
       <c r="M33" s="29"/>
       <c r="N33" s="29"/>
       <c r="O33" s="30"/>
-      <c r="P33" s="31"/>
+      <c r="P33" s="51"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="33"/>
+      <c r="R33" s="31"/>
       <c r="S33" s="30"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="34"/>
-      <c r="V33" s="35"/>
+      <c r="T33" s="31"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="46"/>
       <c r="W33" s="24"/>
       <c r="X33" s="7"/>
       <c r="Y33" s="7"/>
@@ -4957,13 +4975,13 @@
       <c r="M34" s="29"/>
       <c r="N34" s="29"/>
       <c r="O34" s="30"/>
-      <c r="P34" s="31"/>
+      <c r="P34" s="51"/>
       <c r="Q34" s="32"/>
-      <c r="R34" s="33"/>
+      <c r="R34" s="31"/>
       <c r="S34" s="30"/>
-      <c r="T34" s="33"/>
-      <c r="U34" s="34"/>
-      <c r="V34" s="35"/>
+      <c r="T34" s="31"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="46"/>
       <c r="W34" s="24"/>
       <c r="X34" s="7"/>
       <c r="Y34" s="7"/>
@@ -4992,13 +5010,13 @@
       <c r="M35" s="29"/>
       <c r="N35" s="29"/>
       <c r="O35" s="30"/>
-      <c r="P35" s="31"/>
+      <c r="P35" s="51"/>
       <c r="Q35" s="32"/>
-      <c r="R35" s="33"/>
+      <c r="R35" s="31"/>
       <c r="S35" s="30"/>
-      <c r="T35" s="33"/>
-      <c r="U35" s="34"/>
-      <c r="V35" s="35"/>
+      <c r="T35" s="31"/>
+      <c r="U35" s="45"/>
+      <c r="V35" s="46"/>
       <c r="W35" s="24"/>
       <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
@@ -5027,13 +5045,13 @@
       <c r="M36" s="29"/>
       <c r="N36" s="29"/>
       <c r="O36" s="30"/>
-      <c r="P36" s="31"/>
+      <c r="P36" s="51"/>
       <c r="Q36" s="32"/>
-      <c r="R36" s="33"/>
+      <c r="R36" s="31"/>
       <c r="S36" s="30"/>
-      <c r="T36" s="33"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="35"/>
+      <c r="T36" s="31"/>
+      <c r="U36" s="45"/>
+      <c r="V36" s="46"/>
       <c r="W36" s="24"/>
       <c r="X36" s="7"/>
       <c r="Y36" s="7"/>
@@ -5062,13 +5080,13 @@
       <c r="M37" s="29"/>
       <c r="N37" s="29"/>
       <c r="O37" s="30"/>
-      <c r="P37" s="31"/>
+      <c r="P37" s="51"/>
       <c r="Q37" s="32"/>
-      <c r="R37" s="33"/>
+      <c r="R37" s="31"/>
       <c r="S37" s="30"/>
-      <c r="T37" s="33"/>
-      <c r="U37" s="34"/>
-      <c r="V37" s="35"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="46"/>
       <c r="W37" s="24"/>
       <c r="X37" s="7"/>
       <c r="Y37" s="7"/>
@@ -5097,13 +5115,13 @@
       <c r="M38" s="29"/>
       <c r="N38" s="29"/>
       <c r="O38" s="30"/>
-      <c r="P38" s="31"/>
+      <c r="P38" s="51"/>
       <c r="Q38" s="32"/>
-      <c r="R38" s="33"/>
+      <c r="R38" s="31"/>
       <c r="S38" s="30"/>
-      <c r="T38" s="33"/>
-      <c r="U38" s="34"/>
-      <c r="V38" s="35"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="46"/>
       <c r="W38" s="24"/>
       <c r="X38" s="7"/>
       <c r="Y38" s="7"/>
@@ -5132,13 +5150,13 @@
       <c r="M39" s="29"/>
       <c r="N39" s="29"/>
       <c r="O39" s="30"/>
-      <c r="P39" s="31"/>
+      <c r="P39" s="51"/>
       <c r="Q39" s="32"/>
-      <c r="R39" s="33"/>
+      <c r="R39" s="31"/>
       <c r="S39" s="30"/>
-      <c r="T39" s="33"/>
-      <c r="U39" s="34"/>
-      <c r="V39" s="35"/>
+      <c r="T39" s="31"/>
+      <c r="U39" s="45"/>
+      <c r="V39" s="46"/>
       <c r="W39" s="24"/>
       <c r="X39" s="7"/>
       <c r="Y39" s="7"/>
@@ -5167,13 +5185,13 @@
       <c r="M40" s="29"/>
       <c r="N40" s="29"/>
       <c r="O40" s="30"/>
-      <c r="P40" s="31"/>
+      <c r="P40" s="51"/>
       <c r="Q40" s="32"/>
-      <c r="R40" s="33"/>
+      <c r="R40" s="31"/>
       <c r="S40" s="30"/>
-      <c r="T40" s="33"/>
-      <c r="U40" s="34"/>
-      <c r="V40" s="35"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="46"/>
       <c r="W40" s="24"/>
       <c r="X40" s="7"/>
       <c r="Y40" s="7"/>
@@ -5202,13 +5220,13 @@
       <c r="M41" s="29"/>
       <c r="N41" s="29"/>
       <c r="O41" s="30"/>
-      <c r="P41" s="31"/>
+      <c r="P41" s="51"/>
       <c r="Q41" s="32"/>
-      <c r="R41" s="33"/>
+      <c r="R41" s="31"/>
       <c r="S41" s="30"/>
-      <c r="T41" s="33"/>
-      <c r="U41" s="34"/>
-      <c r="V41" s="35"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="45"/>
+      <c r="V41" s="46"/>
       <c r="W41" s="24"/>
       <c r="X41" s="7"/>
       <c r="Y41" s="7"/>
@@ -5237,13 +5255,13 @@
       <c r="M42" s="29"/>
       <c r="N42" s="29"/>
       <c r="O42" s="30"/>
-      <c r="P42" s="31"/>
+      <c r="P42" s="51"/>
       <c r="Q42" s="32"/>
-      <c r="R42" s="33"/>
+      <c r="R42" s="31"/>
       <c r="S42" s="30"/>
-      <c r="T42" s="33"/>
-      <c r="U42" s="34"/>
-      <c r="V42" s="35"/>
+      <c r="T42" s="31"/>
+      <c r="U42" s="45"/>
+      <c r="V42" s="46"/>
       <c r="W42" s="24"/>
       <c r="X42" s="7"/>
       <c r="Y42" s="7"/>
@@ -5272,13 +5290,13 @@
       <c r="M43" s="29"/>
       <c r="N43" s="29"/>
       <c r="O43" s="30"/>
-      <c r="P43" s="31"/>
+      <c r="P43" s="51"/>
       <c r="Q43" s="32"/>
-      <c r="R43" s="33"/>
+      <c r="R43" s="31"/>
       <c r="S43" s="30"/>
-      <c r="T43" s="33"/>
-      <c r="U43" s="34"/>
-      <c r="V43" s="35"/>
+      <c r="T43" s="31"/>
+      <c r="U43" s="45"/>
+      <c r="V43" s="46"/>
       <c r="W43" s="24"/>
       <c r="X43" s="7"/>
       <c r="Y43" s="7"/>
@@ -5307,13 +5325,13 @@
       <c r="M44" s="29"/>
       <c r="N44" s="29"/>
       <c r="O44" s="30"/>
-      <c r="P44" s="31"/>
+      <c r="P44" s="51"/>
       <c r="Q44" s="32"/>
-      <c r="R44" s="33"/>
+      <c r="R44" s="31"/>
       <c r="S44" s="30"/>
-      <c r="T44" s="33"/>
-      <c r="U44" s="34"/>
-      <c r="V44" s="35"/>
+      <c r="T44" s="31"/>
+      <c r="U44" s="45"/>
+      <c r="V44" s="46"/>
       <c r="W44" s="24"/>
       <c r="X44" s="7"/>
       <c r="Y44" s="7"/>
@@ -5342,13 +5360,13 @@
       <c r="M45" s="29"/>
       <c r="N45" s="29"/>
       <c r="O45" s="30"/>
-      <c r="P45" s="31"/>
+      <c r="P45" s="51"/>
       <c r="Q45" s="32"/>
-      <c r="R45" s="33"/>
+      <c r="R45" s="31"/>
       <c r="S45" s="30"/>
-      <c r="T45" s="33"/>
-      <c r="U45" s="34"/>
-      <c r="V45" s="35"/>
+      <c r="T45" s="31"/>
+      <c r="U45" s="45"/>
+      <c r="V45" s="46"/>
       <c r="W45" s="24"/>
       <c r="X45" s="7"/>
       <c r="Y45" s="7"/>
@@ -5377,13 +5395,13 @@
       <c r="M46" s="29"/>
       <c r="N46" s="29"/>
       <c r="O46" s="30"/>
-      <c r="P46" s="31"/>
+      <c r="P46" s="51"/>
       <c r="Q46" s="32"/>
-      <c r="R46" s="33"/>
+      <c r="R46" s="31"/>
       <c r="S46" s="30"/>
-      <c r="T46" s="33"/>
-      <c r="U46" s="34"/>
-      <c r="V46" s="35"/>
+      <c r="T46" s="31"/>
+      <c r="U46" s="45"/>
+      <c r="V46" s="46"/>
       <c r="W46" s="24"/>
       <c r="X46" s="7"/>
       <c r="Y46" s="7"/>
@@ -5412,13 +5430,13 @@
       <c r="M47" s="29"/>
       <c r="N47" s="29"/>
       <c r="O47" s="30"/>
-      <c r="P47" s="31"/>
+      <c r="P47" s="51"/>
       <c r="Q47" s="32"/>
-      <c r="R47" s="33"/>
+      <c r="R47" s="31"/>
       <c r="S47" s="30"/>
-      <c r="T47" s="33"/>
-      <c r="U47" s="34"/>
-      <c r="V47" s="35"/>
+      <c r="T47" s="31"/>
+      <c r="U47" s="45"/>
+      <c r="V47" s="46"/>
       <c r="W47" s="24"/>
       <c r="X47" s="7"/>
       <c r="Y47" s="7"/>
@@ -5447,13 +5465,13 @@
       <c r="M48" s="29"/>
       <c r="N48" s="29"/>
       <c r="O48" s="30"/>
-      <c r="P48" s="31"/>
+      <c r="P48" s="51"/>
       <c r="Q48" s="32"/>
-      <c r="R48" s="33"/>
+      <c r="R48" s="31"/>
       <c r="S48" s="30"/>
-      <c r="T48" s="33"/>
-      <c r="U48" s="34"/>
-      <c r="V48" s="35"/>
+      <c r="T48" s="31"/>
+      <c r="U48" s="45"/>
+      <c r="V48" s="46"/>
       <c r="W48" s="24"/>
       <c r="X48" s="7"/>
       <c r="Y48" s="7"/>
@@ -5482,13 +5500,13 @@
       <c r="M49" s="29"/>
       <c r="N49" s="29"/>
       <c r="O49" s="30"/>
-      <c r="P49" s="31"/>
+      <c r="P49" s="51"/>
       <c r="Q49" s="32"/>
-      <c r="R49" s="33"/>
+      <c r="R49" s="31"/>
       <c r="S49" s="30"/>
-      <c r="T49" s="33"/>
-      <c r="U49" s="34"/>
-      <c r="V49" s="35"/>
+      <c r="T49" s="31"/>
+      <c r="U49" s="45"/>
+      <c r="V49" s="46"/>
       <c r="W49" s="24"/>
       <c r="X49" s="7"/>
       <c r="Y49" s="7"/>
@@ -5517,13 +5535,13 @@
       <c r="M50" s="29"/>
       <c r="N50" s="29"/>
       <c r="O50" s="30"/>
-      <c r="P50" s="31"/>
+      <c r="P50" s="51"/>
       <c r="Q50" s="32"/>
-      <c r="R50" s="33"/>
+      <c r="R50" s="31"/>
       <c r="S50" s="30"/>
-      <c r="T50" s="33"/>
-      <c r="U50" s="34"/>
-      <c r="V50" s="35"/>
+      <c r="T50" s="31"/>
+      <c r="U50" s="45"/>
+      <c r="V50" s="46"/>
       <c r="W50" s="24"/>
       <c r="X50" s="7"/>
       <c r="Y50" s="7"/>
@@ -5552,13 +5570,13 @@
       <c r="M51" s="29"/>
       <c r="N51" s="29"/>
       <c r="O51" s="30"/>
-      <c r="P51" s="31"/>
+      <c r="P51" s="51"/>
       <c r="Q51" s="32"/>
-      <c r="R51" s="33"/>
+      <c r="R51" s="31"/>
       <c r="S51" s="30"/>
-      <c r="T51" s="33"/>
-      <c r="U51" s="34"/>
-      <c r="V51" s="35"/>
+      <c r="T51" s="31"/>
+      <c r="U51" s="45"/>
+      <c r="V51" s="46"/>
       <c r="W51" s="3"/>
     </row>
     <row r="52" spans="1:30">
@@ -5580,13 +5598,13 @@
       <c r="M52" s="29"/>
       <c r="N52" s="29"/>
       <c r="O52" s="30"/>
-      <c r="P52" s="31"/>
+      <c r="P52" s="51"/>
       <c r="Q52" s="32"/>
-      <c r="R52" s="33"/>
+      <c r="R52" s="31"/>
       <c r="S52" s="30"/>
-      <c r="T52" s="33"/>
-      <c r="U52" s="34"/>
-      <c r="V52" s="35"/>
+      <c r="T52" s="31"/>
+      <c r="U52" s="45"/>
+      <c r="V52" s="46"/>
       <c r="W52" s="3"/>
     </row>
     <row r="53" spans="1:30">
@@ -5608,13 +5626,13 @@
       <c r="M53" s="29"/>
       <c r="N53" s="29"/>
       <c r="O53" s="30"/>
-      <c r="P53" s="31"/>
+      <c r="P53" s="51"/>
       <c r="Q53" s="32"/>
-      <c r="R53" s="33"/>
+      <c r="R53" s="31"/>
       <c r="S53" s="30"/>
-      <c r="T53" s="33"/>
-      <c r="U53" s="34"/>
-      <c r="V53" s="35"/>
+      <c r="T53" s="31"/>
+      <c r="U53" s="45"/>
+      <c r="V53" s="46"/>
       <c r="W53" s="3"/>
     </row>
     <row r="54" spans="1:30">
@@ -5636,13 +5654,13 @@
       <c r="M54" s="29"/>
       <c r="N54" s="29"/>
       <c r="O54" s="30"/>
-      <c r="P54" s="31"/>
+      <c r="P54" s="51"/>
       <c r="Q54" s="32"/>
-      <c r="R54" s="33"/>
+      <c r="R54" s="31"/>
       <c r="S54" s="30"/>
-      <c r="T54" s="33"/>
-      <c r="U54" s="34"/>
-      <c r="V54" s="35"/>
+      <c r="T54" s="31"/>
+      <c r="U54" s="45"/>
+      <c r="V54" s="46"/>
       <c r="W54" s="3"/>
     </row>
     <row r="55" spans="1:30">
@@ -5664,13 +5682,13 @@
       <c r="M55" s="29"/>
       <c r="N55" s="29"/>
       <c r="O55" s="30"/>
-      <c r="P55" s="31"/>
+      <c r="P55" s="51"/>
       <c r="Q55" s="32"/>
-      <c r="R55" s="33"/>
+      <c r="R55" s="31"/>
       <c r="S55" s="30"/>
-      <c r="T55" s="33"/>
-      <c r="U55" s="34"/>
-      <c r="V55" s="35"/>
+      <c r="T55" s="31"/>
+      <c r="U55" s="45"/>
+      <c r="V55" s="46"/>
       <c r="W55" s="3"/>
     </row>
     <row r="56" spans="1:30">
@@ -5692,13 +5710,13 @@
       <c r="M56" s="29"/>
       <c r="N56" s="29"/>
       <c r="O56" s="30"/>
-      <c r="P56" s="31"/>
+      <c r="P56" s="51"/>
       <c r="Q56" s="32"/>
-      <c r="R56" s="33"/>
+      <c r="R56" s="31"/>
       <c r="S56" s="30"/>
-      <c r="T56" s="33"/>
-      <c r="U56" s="34"/>
-      <c r="V56" s="35"/>
+      <c r="T56" s="31"/>
+      <c r="U56" s="45"/>
+      <c r="V56" s="46"/>
       <c r="W56" s="3"/>
       <c r="AD56" s="7"/>
     </row>
@@ -5721,13 +5739,13 @@
       <c r="M57" s="29"/>
       <c r="N57" s="29"/>
       <c r="O57" s="30"/>
-      <c r="P57" s="31"/>
+      <c r="P57" s="51"/>
       <c r="Q57" s="32"/>
-      <c r="R57" s="33"/>
+      <c r="R57" s="31"/>
       <c r="S57" s="30"/>
-      <c r="T57" s="33"/>
-      <c r="U57" s="34"/>
-      <c r="V57" s="35"/>
+      <c r="T57" s="31"/>
+      <c r="U57" s="45"/>
+      <c r="V57" s="46"/>
       <c r="W57" s="3"/>
       <c r="AD57" s="7"/>
     </row>
@@ -5750,13 +5768,13 @@
       <c r="M58" s="29"/>
       <c r="N58" s="29"/>
       <c r="O58" s="30"/>
-      <c r="P58" s="31"/>
+      <c r="P58" s="51"/>
       <c r="Q58" s="32"/>
-      <c r="R58" s="33"/>
+      <c r="R58" s="31"/>
       <c r="S58" s="30"/>
-      <c r="T58" s="33"/>
-      <c r="U58" s="34"/>
-      <c r="V58" s="35"/>
+      <c r="T58" s="31"/>
+      <c r="U58" s="45"/>
+      <c r="V58" s="46"/>
       <c r="W58" s="3"/>
       <c r="AD58" s="7"/>
     </row>
@@ -5779,13 +5797,13 @@
       <c r="M59" s="29"/>
       <c r="N59" s="29"/>
       <c r="O59" s="30"/>
-      <c r="P59" s="31"/>
+      <c r="P59" s="51"/>
       <c r="Q59" s="32"/>
-      <c r="R59" s="33"/>
+      <c r="R59" s="31"/>
       <c r="S59" s="30"/>
-      <c r="T59" s="33"/>
-      <c r="U59" s="34"/>
-      <c r="V59" s="35"/>
+      <c r="T59" s="31"/>
+      <c r="U59" s="45"/>
+      <c r="V59" s="46"/>
       <c r="W59" s="3"/>
       <c r="AD59" s="7"/>
     </row>
@@ -5808,13 +5826,13 @@
       <c r="M60" s="29"/>
       <c r="N60" s="29"/>
       <c r="O60" s="30"/>
-      <c r="P60" s="31"/>
+      <c r="P60" s="51"/>
       <c r="Q60" s="32"/>
-      <c r="R60" s="33"/>
+      <c r="R60" s="31"/>
       <c r="S60" s="30"/>
-      <c r="T60" s="33"/>
-      <c r="U60" s="34"/>
-      <c r="V60" s="35"/>
+      <c r="T60" s="31"/>
+      <c r="U60" s="45"/>
+      <c r="V60" s="46"/>
       <c r="W60" s="3"/>
       <c r="AD60" s="7"/>
     </row>
@@ -5837,13 +5855,13 @@
       <c r="M61" s="29"/>
       <c r="N61" s="29"/>
       <c r="O61" s="30"/>
-      <c r="P61" s="31"/>
+      <c r="P61" s="51"/>
       <c r="Q61" s="32"/>
-      <c r="R61" s="33"/>
+      <c r="R61" s="31"/>
       <c r="S61" s="30"/>
-      <c r="T61" s="33"/>
-      <c r="U61" s="34"/>
-      <c r="V61" s="35"/>
+      <c r="T61" s="31"/>
+      <c r="U61" s="45"/>
+      <c r="V61" s="46"/>
       <c r="W61" s="3"/>
       <c r="AD61" s="7"/>
     </row>
@@ -5866,13 +5884,13 @@
       <c r="M62" s="29"/>
       <c r="N62" s="29"/>
       <c r="O62" s="30"/>
-      <c r="P62" s="31"/>
+      <c r="P62" s="51"/>
       <c r="Q62" s="32"/>
-      <c r="R62" s="33"/>
+      <c r="R62" s="31"/>
       <c r="S62" s="30"/>
-      <c r="T62" s="33"/>
-      <c r="U62" s="34"/>
-      <c r="V62" s="35"/>
+      <c r="T62" s="31"/>
+      <c r="U62" s="45"/>
+      <c r="V62" s="46"/>
       <c r="W62" s="3"/>
       <c r="AD62" s="7"/>
     </row>
@@ -5895,13 +5913,13 @@
       <c r="M63" s="29"/>
       <c r="N63" s="29"/>
       <c r="O63" s="30"/>
-      <c r="P63" s="31"/>
+      <c r="P63" s="51"/>
       <c r="Q63" s="32"/>
-      <c r="R63" s="33"/>
+      <c r="R63" s="31"/>
       <c r="S63" s="30"/>
-      <c r="T63" s="33"/>
-      <c r="U63" s="34"/>
-      <c r="V63" s="35"/>
+      <c r="T63" s="31"/>
+      <c r="U63" s="45"/>
+      <c r="V63" s="46"/>
       <c r="AD63" s="7"/>
     </row>
     <row r="64" spans="1:30">
@@ -5923,13 +5941,13 @@
       <c r="M64" s="29"/>
       <c r="N64" s="29"/>
       <c r="O64" s="30"/>
-      <c r="P64" s="31"/>
+      <c r="P64" s="51"/>
       <c r="Q64" s="32"/>
-      <c r="R64" s="33"/>
+      <c r="R64" s="31"/>
       <c r="S64" s="30"/>
-      <c r="T64" s="33"/>
-      <c r="U64" s="34"/>
-      <c r="V64" s="35"/>
+      <c r="T64" s="31"/>
+      <c r="U64" s="45"/>
+      <c r="V64" s="46"/>
       <c r="AD64" s="7"/>
     </row>
     <row r="65" spans="1:30">
@@ -5951,13 +5969,13 @@
       <c r="M65" s="29"/>
       <c r="N65" s="29"/>
       <c r="O65" s="30"/>
-      <c r="P65" s="31"/>
+      <c r="P65" s="51"/>
       <c r="Q65" s="32"/>
-      <c r="R65" s="33"/>
+      <c r="R65" s="31"/>
       <c r="S65" s="30"/>
-      <c r="T65" s="33"/>
-      <c r="U65" s="34"/>
-      <c r="V65" s="35"/>
+      <c r="T65" s="31"/>
+      <c r="U65" s="45"/>
+      <c r="V65" s="46"/>
       <c r="AD65" s="7"/>
     </row>
     <row r="66" spans="1:30">
@@ -5979,13 +5997,13 @@
       <c r="M66" s="29"/>
       <c r="N66" s="29"/>
       <c r="O66" s="30"/>
-      <c r="P66" s="36"/>
+      <c r="P66" s="52"/>
       <c r="Q66" s="32"/>
-      <c r="R66" s="33"/>
+      <c r="R66" s="31"/>
       <c r="S66" s="30"/>
-      <c r="T66" s="33"/>
-      <c r="U66" s="34"/>
-      <c r="V66" s="35"/>
+      <c r="T66" s="31"/>
+      <c r="U66" s="45"/>
+      <c r="V66" s="46"/>
       <c r="AD66" s="7"/>
     </row>
     <row r="67" spans="1:30">
@@ -6007,13 +6025,13 @@
       <c r="M67" s="29"/>
       <c r="N67" s="29"/>
       <c r="O67" s="30"/>
-      <c r="P67" s="31"/>
+      <c r="P67" s="51"/>
       <c r="Q67" s="32"/>
-      <c r="R67" s="33"/>
+      <c r="R67" s="31"/>
       <c r="S67" s="30"/>
-      <c r="T67" s="33"/>
-      <c r="U67" s="34"/>
-      <c r="V67" s="35"/>
+      <c r="T67" s="31"/>
+      <c r="U67" s="45"/>
+      <c r="V67" s="46"/>
       <c r="AD67" s="7"/>
     </row>
     <row r="68" spans="1:30">
@@ -6035,13 +6053,13 @@
       <c r="M68" s="29"/>
       <c r="N68" s="29"/>
       <c r="O68" s="30"/>
-      <c r="P68" s="31"/>
-      <c r="Q68" s="37"/>
-      <c r="R68" s="33"/>
+      <c r="P68" s="51"/>
+      <c r="Q68" s="32"/>
+      <c r="R68" s="31"/>
       <c r="S68" s="30"/>
-      <c r="T68" s="33"/>
-      <c r="U68" s="34"/>
-      <c r="V68" s="35"/>
+      <c r="T68" s="31"/>
+      <c r="U68" s="45"/>
+      <c r="V68" s="46"/>
       <c r="AD68" s="7"/>
     </row>
     <row r="69" spans="1:30">
@@ -6063,13 +6081,13 @@
       <c r="M69" s="29"/>
       <c r="N69" s="29"/>
       <c r="O69" s="30"/>
-      <c r="P69" s="31"/>
+      <c r="P69" s="51"/>
       <c r="Q69" s="32"/>
-      <c r="R69" s="33"/>
+      <c r="R69" s="31"/>
       <c r="S69" s="30"/>
-      <c r="T69" s="33"/>
-      <c r="U69" s="34"/>
-      <c r="V69" s="35"/>
+      <c r="T69" s="31"/>
+      <c r="U69" s="45"/>
+      <c r="V69" s="46"/>
       <c r="AD69" s="7"/>
     </row>
     <row r="70" spans="1:30">
@@ -6091,13 +6109,13 @@
       <c r="M70" s="29"/>
       <c r="N70" s="29"/>
       <c r="O70" s="30"/>
-      <c r="P70" s="31"/>
+      <c r="P70" s="51"/>
       <c r="Q70" s="32"/>
-      <c r="R70" s="33"/>
+      <c r="R70" s="31"/>
       <c r="S70" s="30"/>
-      <c r="T70" s="33"/>
-      <c r="U70" s="34"/>
-      <c r="V70" s="35"/>
+      <c r="T70" s="31"/>
+      <c r="U70" s="45"/>
+      <c r="V70" s="46"/>
       <c r="AD70" s="7"/>
     </row>
     <row r="71" spans="1:30">
@@ -6119,13 +6137,13 @@
       <c r="M71" s="29"/>
       <c r="N71" s="29"/>
       <c r="O71" s="30"/>
-      <c r="P71" s="31"/>
+      <c r="P71" s="51"/>
       <c r="Q71" s="32"/>
-      <c r="R71" s="33"/>
+      <c r="R71" s="31"/>
       <c r="S71" s="30"/>
-      <c r="T71" s="33"/>
-      <c r="U71" s="34"/>
-      <c r="V71" s="35"/>
+      <c r="T71" s="31"/>
+      <c r="U71" s="45"/>
+      <c r="V71" s="46"/>
       <c r="AD71" s="7"/>
     </row>
     <row r="72" spans="1:30">
@@ -6147,13 +6165,13 @@
       <c r="M72" s="29"/>
       <c r="N72" s="29"/>
       <c r="O72" s="30"/>
-      <c r="P72" s="31"/>
+      <c r="P72" s="51"/>
       <c r="Q72" s="32"/>
-      <c r="R72" s="33"/>
+      <c r="R72" s="31"/>
       <c r="S72" s="30"/>
-      <c r="T72" s="33"/>
-      <c r="U72" s="34"/>
-      <c r="V72" s="35"/>
+      <c r="T72" s="31"/>
+      <c r="U72" s="45"/>
+      <c r="V72" s="46"/>
       <c r="AD72" s="7"/>
     </row>
     <row r="73" spans="1:30">
@@ -6175,13 +6193,13 @@
       <c r="M73" s="29"/>
       <c r="N73" s="29"/>
       <c r="O73" s="30"/>
-      <c r="P73" s="31"/>
+      <c r="P73" s="51"/>
       <c r="Q73" s="32"/>
-      <c r="R73" s="33"/>
+      <c r="R73" s="31"/>
       <c r="S73" s="30"/>
-      <c r="T73" s="33"/>
-      <c r="U73" s="34"/>
-      <c r="V73" s="35"/>
+      <c r="T73" s="31"/>
+      <c r="U73" s="45"/>
+      <c r="V73" s="46"/>
       <c r="AD73" s="7"/>
     </row>
     <row r="74" spans="1:30">
@@ -6203,18 +6221,72 @@
       <c r="M74" s="29"/>
       <c r="N74" s="29"/>
       <c r="O74" s="30"/>
-      <c r="P74" s="31"/>
+      <c r="P74" s="51"/>
       <c r="Q74" s="32"/>
-      <c r="R74" s="33"/>
+      <c r="R74" s="31"/>
       <c r="S74" s="30"/>
-      <c r="T74" s="33"/>
-      <c r="U74" s="34"/>
-      <c r="V74" s="35"/>
+      <c r="T74" s="31"/>
+      <c r="U74" s="45"/>
+      <c r="V74" s="46"/>
       <c r="AD74" s="7"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="70">
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="U32:V32"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="U37:V37"/>
+    <mergeCell ref="U38:V38"/>
+    <mergeCell ref="U39:V39"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="U43:V43"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="U46:V46"/>
+    <mergeCell ref="U47:V47"/>
+    <mergeCell ref="U48:V48"/>
+    <mergeCell ref="U49:V49"/>
+    <mergeCell ref="U50:V50"/>
+    <mergeCell ref="U51:V51"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U53:V53"/>
+    <mergeCell ref="U54:V54"/>
+    <mergeCell ref="U55:V55"/>
+    <mergeCell ref="U56:V56"/>
+    <mergeCell ref="U57:V57"/>
+    <mergeCell ref="U58:V58"/>
     <mergeCell ref="U71:V71"/>
     <mergeCell ref="U72:V72"/>
     <mergeCell ref="U73:V73"/>
@@ -6231,60 +6303,6 @@
     <mergeCell ref="U61:V61"/>
     <mergeCell ref="U62:V62"/>
     <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U53:V53"/>
-    <mergeCell ref="U54:V54"/>
-    <mergeCell ref="U55:V55"/>
-    <mergeCell ref="U56:V56"/>
-    <mergeCell ref="U57:V57"/>
-    <mergeCell ref="U58:V58"/>
-    <mergeCell ref="U47:V47"/>
-    <mergeCell ref="U48:V48"/>
-    <mergeCell ref="U49:V49"/>
-    <mergeCell ref="U50:V50"/>
-    <mergeCell ref="U51:V51"/>
-    <mergeCell ref="U52:V52"/>
-    <mergeCell ref="U41:V41"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="U43:V43"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="U46:V46"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="U37:V37"/>
-    <mergeCell ref="U38:V38"/>
-    <mergeCell ref="U39:V39"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="U32:V32"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="R27:T27 R30:T30 Q31:S31 F58:F63 G29:G30 F31:G31 G56:G63 F25:G28 F51:G55 D25:E31 D51:E63 D64:G74 D32:G50 C31:C74 Q28:T29 Q51:T64 Q67:T68 Q72:T74 Q10:T25 Q9 C6:U6 P9:P74 O9:O25 H9:N74 C9:C29 D9:G24 C8:U8">

</xml_diff>